<commit_message>
Dodano zapisywanie talii kart z pliku excel
</commit_message>
<xml_diff>
--- a/backend/DigitalWars_SzablonKart.xlsx
+++ b/backend/DigitalWars_SzablonKart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ITM_ProjektZespo-owy-Grupson_Project\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92286E68-7C05-4299-A21E-7450877BF575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47FCD6B-D4D9-4928-BDD0-C14A0A67B102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Decisions" sheetId="1" r:id="rId1"/>
@@ -4474,8 +4474,8 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4682,8 +4682,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="15">
-        <f t="shared" si="0"/>
-        <v>113</v>
+        <v>201</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>100</v>
@@ -4698,7 +4697,7 @@
     <row r="15" spans="1:4">
       <c r="A15" s="15">
         <f t="shared" si="0"/>
-        <v>114</v>
+        <v>202</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>102</v>
@@ -4713,7 +4712,7 @@
     <row r="16" spans="1:4">
       <c r="A16" s="15">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>203</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>104</v>
@@ -4728,7 +4727,7 @@
     <row r="17" spans="1:4">
       <c r="A17" s="15">
         <f t="shared" si="0"/>
-        <v>116</v>
+        <v>204</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>106</v>
@@ -4743,7 +4742,7 @@
     <row r="18" spans="1:4">
       <c r="A18" s="15">
         <f t="shared" si="0"/>
-        <v>117</v>
+        <v>205</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>108</v>
@@ -4758,7 +4757,7 @@
     <row r="19" spans="1:4">
       <c r="A19" s="15">
         <f t="shared" si="0"/>
-        <v>118</v>
+        <v>206</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>110</v>
@@ -4773,7 +4772,7 @@
     <row r="20" spans="1:4">
       <c r="A20" s="15">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>207</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>112</v>
@@ -4788,7 +4787,7 @@
     <row r="21" spans="1:4">
       <c r="A21" s="15">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>208</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>114</v>
@@ -4803,7 +4802,7 @@
     <row r="22" spans="1:4">
       <c r="A22" s="15">
         <f t="shared" si="0"/>
-        <v>121</v>
+        <v>209</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>116</v>
@@ -4818,7 +4817,7 @@
     <row r="23" spans="1:4">
       <c r="A23" s="15">
         <f t="shared" si="0"/>
-        <v>122</v>
+        <v>210</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>118</v>
@@ -4833,7 +4832,7 @@
     <row r="24" spans="1:4">
       <c r="A24" s="15">
         <f t="shared" si="0"/>
-        <v>123</v>
+        <v>211</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>120</v>
@@ -4848,7 +4847,7 @@
     <row r="25" spans="1:4">
       <c r="A25" s="15">
         <f t="shared" si="0"/>
-        <v>124</v>
+        <v>212</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>122</v>
@@ -4863,7 +4862,7 @@
     <row r="26" spans="1:4">
       <c r="A26" s="15">
         <f t="shared" si="0"/>
-        <v>125</v>
+        <v>213</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>124</v>
@@ -4878,7 +4877,7 @@
     <row r="27" spans="1:4">
       <c r="A27" s="15">
         <f t="shared" si="0"/>
-        <v>126</v>
+        <v>214</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>126</v>
@@ -4893,7 +4892,7 @@
     <row r="28" spans="1:4">
       <c r="A28" s="15">
         <f t="shared" si="0"/>
-        <v>127</v>
+        <v>215</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>128</v>
@@ -4908,7 +4907,7 @@
     <row r="29" spans="1:4">
       <c r="A29" s="15">
         <f t="shared" si="0"/>
-        <v>128</v>
+        <v>216</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>130</v>
@@ -4923,7 +4922,7 @@
     <row r="30" spans="1:4">
       <c r="A30" s="15">
         <f t="shared" si="0"/>
-        <v>129</v>
+        <v>217</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>132</v>
@@ -4938,7 +4937,7 @@
     <row r="31" spans="1:4">
       <c r="A31" s="15">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>218</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>134</v>
@@ -4953,7 +4952,7 @@
     <row r="32" spans="1:4">
       <c r="A32" s="15">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>219</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>136</v>
@@ -4968,7 +4967,7 @@
     <row r="33" spans="1:4">
       <c r="A33" s="15">
         <f t="shared" si="0"/>
-        <v>132</v>
+        <v>220</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>138</v>
@@ -4983,7 +4982,7 @@
     <row r="34" spans="1:4">
       <c r="A34" s="15">
         <f t="shared" si="0"/>
-        <v>133</v>
+        <v>221</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>140</v>
@@ -4998,7 +4997,7 @@
     <row r="35" spans="1:4">
       <c r="A35" s="15">
         <f t="shared" si="0"/>
-        <v>134</v>
+        <v>222</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>142</v>
@@ -5012,7 +5011,6 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="15">
-        <f>A35+1</f>
         <v>135</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -7925,7 +7923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>